<commit_message>
updated jumla script to combine datasets
</commit_message>
<xml_diff>
--- a/scripts/resources/sign_index.xlsx
+++ b/scripts/resources/sign_index.xlsx
@@ -1254,7 +1254,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1265,6 +1265,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1298,13 +1304,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">

</xml_diff>